<commit_message>
Added type restrictions for the methods
</commit_message>
<xml_diff>
--- a/gRNASequences.xlsx
+++ b/gRNASequences.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10315"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sophiewu/Documents/ReitmanLab/RCAS-gRNA-PDGFB_Cloning/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E805D2B3-40DC-1243-BFBB-B0F73C6E2F8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB656E8B-F049-AE41-A429-E9AF8E4AB935}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5580" yWindow="2300" windowWidth="27640" windowHeight="16940" xr2:uid="{C203D3CC-8220-C54E-9ADD-B0E6BCB450A6}"/>
+    <workbookView xWindow="15480" yWindow="2180" windowWidth="27640" windowHeight="16940" xr2:uid="{C203D3CC-8220-C54E-9ADD-B0E6BCB450A6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -119,9 +119,6 @@
     <t>GATGGACCACAGGTGGCACA</t>
   </si>
   <si>
-    <t>AAGTCTGAGAAGCAAAGTAA</t>
-  </si>
-  <si>
     <t>GTAAAGGAACATGTAACGAC</t>
   </si>
   <si>
@@ -180,6 +177,9 @@
   </si>
   <si>
     <t>sgRNA Sequence (5'-3')</t>
+  </si>
+  <si>
+    <t>TAGTTCCCATAGCTGCCAGG</t>
   </si>
 </sst>
 </file>
@@ -587,7 +587,7 @@
   <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L21" sqref="L21"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -600,7 +600,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17">
@@ -632,7 +632,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>27</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="17">
@@ -640,7 +640,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="17">
@@ -648,7 +648,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="17">
@@ -656,7 +656,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="17">
@@ -664,7 +664,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="17">
@@ -672,7 +672,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="17">
@@ -680,7 +680,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="17">
@@ -688,7 +688,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="17">
@@ -696,7 +696,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="17">
@@ -704,7 +704,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="17">
@@ -712,7 +712,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="17">
@@ -720,7 +720,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="17">
@@ -728,7 +728,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="17">
@@ -736,7 +736,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="17">
@@ -744,7 +744,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="17">
@@ -752,7 +752,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="17">
@@ -760,7 +760,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="17">
@@ -768,7 +768,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="17">
@@ -776,7 +776,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="17">
@@ -784,7 +784,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added a docstring to one of the methods
</commit_message>
<xml_diff>
--- a/gRNASequences.xlsx
+++ b/gRNASequences.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sophiewu/Documents/ReitmanLab/RCAS-gRNA-PDGFB_Cloning/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB656E8B-F049-AE41-A429-E9AF8E4AB935}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A11537A-ED4A-1D44-B1C4-FDDB4BB62F7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="15480" yWindow="2180" windowWidth="27640" windowHeight="16940" xr2:uid="{C203D3CC-8220-C54E-9ADD-B0E6BCB450A6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
   <si>
     <t>Gene</t>
   </si>
@@ -180,6 +180,18 @@
   </si>
   <si>
     <t>TAGTTCCCATAGCTGCCAGG</t>
+  </si>
+  <si>
+    <t>ARID1A</t>
+  </si>
+  <si>
+    <t>ARID1B</t>
+  </si>
+  <si>
+    <t>TCAATCGATGATCTCCCCAT</t>
+  </si>
+  <si>
+    <t>CCGCAGTACGGACAGCAAGC</t>
   </si>
 </sst>
 </file>
@@ -584,10 +596,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BE072B7-896A-3A42-8248-8542863A1765}">
-  <dimension ref="A1:B24"/>
+  <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -787,6 +799,22 @@
         <v>45</v>
       </c>
     </row>
+    <row r="25" spans="1:2" ht="17">
+      <c r="A25" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="17">
+      <c r="A26" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>